<commit_message>
GPLIM-4712: Added tests for missing data and malformed numbers.
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryPooledTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryPooledTest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="166">
   <si>
     <t>Sample Kit Shipping Information</t>
   </si>
@@ -2097,8 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AL28" sqref="AL28"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2535,8 +2535,8 @@
       <c r="W27" s="45">
         <v>457457</v>
       </c>
-      <c r="X27" s="45" t="s">
-        <v>150</v>
+      <c r="X27" s="45">
+        <v>100</v>
       </c>
       <c r="Y27" s="45">
         <v>345345</v>

</xml_diff>

<commit_message>
GPLIM-4712 liquibase and more test fixes
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryPooledTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryPooledTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28000" windowHeight="7460"/>
+    <workbookView xWindow="1720" yWindow="1160" windowWidth="17920" windowHeight="7460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,9 +475,6 @@
     <t>DDDSS2244</t>
   </si>
   <si>
-    <t>4442SFF6</t>
-  </si>
-  <si>
     <t>ACAGTCATAT</t>
   </si>
   <si>
@@ -586,9 +583,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>4442SFF7</t>
-  </si>
-  <si>
     <t>AGCATGGA</t>
   </si>
   <si>
@@ -596,6 +590,12 @@
   </si>
   <si>
     <t>Plasmodium_falciparum_3D7</t>
+  </si>
+  <si>
+    <t>4442SFP6</t>
+  </si>
+  <si>
+    <t>4442SFP7</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1347,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1455,6 +1455,20 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1635,7 +1649,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="129">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
     <cellStyle name="20% - Accent1 2 2" xfId="50"/>
     <cellStyle name="20% - Accent1 2 2 2" xfId="84"/>
@@ -1714,6 +1728,20 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Good 2" xfId="31"/>
     <cellStyle name="Heading 1 2" xfId="32"/>
     <cellStyle name="Heading 2 2" xfId="33"/>
@@ -2192,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="AF28" sqref="AF28"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2249,7 +2277,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F5" s="65"/>
       <c r="Z5" s="35"/>
@@ -2259,7 +2287,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Z6" s="35"/>
     </row>
@@ -2268,7 +2296,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Z7" s="35"/>
     </row>
@@ -2277,7 +2305,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Z8" s="35"/>
     </row>
@@ -2297,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Z11" s="35"/>
       <c r="AA11" s="37" t="s">
@@ -2309,7 +2337,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z12" s="35"/>
       <c r="AA12" s="38" t="s">
@@ -2321,7 +2349,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Z13" s="35"/>
       <c r="AA13" s="38" t="s">
@@ -2333,7 +2361,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z14" s="35"/>
       <c r="AA14" s="38" t="s">
@@ -2345,7 +2373,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z15" s="35"/>
       <c r="AA15" s="38" t="s">
@@ -2357,7 +2385,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z16" s="35"/>
       <c r="AA16" s="59" t="s">
@@ -2386,7 +2414,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z19" s="35"/>
       <c r="AA19" s="39"/>
@@ -2396,7 +2424,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Z20" s="35"/>
       <c r="AA20" s="39"/>
@@ -2406,7 +2434,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Z21" s="35"/>
       <c r="AA21" s="39"/>
@@ -2416,7 +2444,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="109" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Z22" s="35"/>
       <c r="AA22" s="39"/>
@@ -2571,19 +2599,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" s="103" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="104" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" s="104" t="s">
         <v>165</v>
       </c>
-      <c r="D27" s="104" t="s">
-        <v>182</v>
-      </c>
-      <c r="E27" s="104" t="s">
-        <v>166</v>
-      </c>
       <c r="F27" s="104" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G27" s="104">
         <v>6</v>
@@ -2592,31 +2620,31 @@
         <v>145</v>
       </c>
       <c r="I27" s="104" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J27" s="104" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="K27" s="45" t="s">
         <v>55</v>
       </c>
       <c r="L27" s="104" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M27" s="104" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N27" s="104" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O27" s="45" t="s">
         <v>57</v>
       </c>
       <c r="P27" s="104" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q27" s="102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R27" s="45">
         <v>1000</v>
@@ -2628,10 +2656,10 @@
         <v>2</v>
       </c>
       <c r="U27" s="102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="V27" s="107" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="W27" s="45">
         <v>77</v>
@@ -2640,46 +2668,46 @@
         <v>100</v>
       </c>
       <c r="Y27" s="102" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z27" s="102" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA27" s="45">
         <v>151</v>
       </c>
       <c r="AB27" s="45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AC27" s="102" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD27" s="45">
+        <v>3</v>
+      </c>
+      <c r="AE27" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="AD27" s="45">
-        <v>8</v>
-      </c>
-      <c r="AE27" s="102" t="s">
+      <c r="AF27" s="102" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG27" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="AF27" s="102" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG27" s="102" t="s">
+      <c r="AH27" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="AH27" s="102" t="s">
+      <c r="AI27" s="108" t="s">
         <v>171</v>
       </c>
-      <c r="AI27" s="108" t="s">
+      <c r="AJ27" s="108" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK27" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="AJ27" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="AK27" s="108" t="s">
-        <v>173</v>
-      </c>
       <c r="AL27" s="108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:40" s="108" customFormat="1" ht="13.5" customHeight="1">
@@ -2687,23 +2715,23 @@
         <v>1</v>
       </c>
       <c r="B28" s="102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" s="103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D28" s="104"/>
       <c r="E28" s="104"/>
       <c r="F28" s="104"/>
       <c r="G28" s="104"/>
       <c r="H28" s="104" t="s">
+        <v>175</v>
+      </c>
+      <c r="I28" s="104" t="s">
         <v>176</v>
       </c>
-      <c r="I28" s="104" t="s">
-        <v>177</v>
-      </c>
       <c r="J28" s="104" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="K28" s="45" t="s">
         <v>55</v>
@@ -2711,13 +2739,13 @@
       <c r="L28" s="104"/>
       <c r="M28" s="104"/>
       <c r="N28" s="104" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O28" s="45" t="s">
         <v>57</v>
       </c>
       <c r="P28" s="104" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q28" s="102"/>
       <c r="R28" s="45">
@@ -2728,7 +2756,7 @@
       </c>
       <c r="T28" s="106"/>
       <c r="U28" s="102" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V28" s="107"/>
       <c r="W28" s="45">
@@ -2739,43 +2767,43 @@
       </c>
       <c r="Y28" s="45"/>
       <c r="Z28" s="102" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AA28" s="45">
         <v>151</v>
       </c>
       <c r="AB28" s="45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AC28" s="102" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD28" s="45">
+        <v>5</v>
+      </c>
+      <c r="AE28" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="AD28" s="45">
-        <v>8</v>
-      </c>
-      <c r="AE28" s="102" t="s">
+      <c r="AF28" s="102" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG28" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="AF28" s="102" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG28" s="102" t="s">
+      <c r="AH28" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="AH28" s="102" t="s">
+      <c r="AI28" s="108" t="s">
         <v>171</v>
       </c>
-      <c r="AI28" s="108" t="s">
+      <c r="AJ28" s="108" t="s">
+        <v>168</v>
+      </c>
+      <c r="AK28" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="AJ28" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="AK28" s="108" t="s">
-        <v>173</v>
-      </c>
       <c r="AL28" s="108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:40" ht="14">

</xml_diff>